<commit_message>
aggiunte motivazioni a data
</commit_message>
<xml_diff>
--- a/data/questions.xlsx
+++ b/data/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcolonghin/Desktop/POM Unimore/Database PCM_Hub/progetto_lingue_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881D8759-9D2F-3542-BC1A-8989E031DBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA08B1D2-9D85-8E4B-91BE-CD666E060022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="23340" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="989">
   <si>
     <t>id</t>
   </si>
@@ -4328,12 +4328,6 @@
 For each example, provide two instances where one and the same personal/relative pronoun occurs in two different syntactic functions (e.g., subject and object) and has two different forms.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no personal/relative pronouns
-- There are no differences in the morphology of personal/relative pronouns depending on their syntactic function
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using different quantifiers, demonstratives and/or definite/indefinite articles.
 For each example, provide two different instances where the quantifier, demonstrative and/or definite/indefinite article occurs in two different syntactic functions (e.g., subject and object) and has two different forms.</t>
   </si>
@@ -4347,12 +4341,6 @@
 For each noun, list all the different available morphological Case distinctions expressing spatial relations.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- the language has no Case morphology on nouns
-- the language has Case morphology on nouns, but there are no morphological Case distinctions expressing spatial relations more complex than stative location, direction, and source
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Provide examples using at least two different nouns.
 For each, list at least two instances of different spatial relations expressed by different prepositions</t>
   </si>
@@ -4364,9 +4352,6 @@
     <t>Do not use an existential construction (e.g. 'There is a dog in the garden') to answer this question.</t>
   </si>
   <si>
-    <t>Provide an example with no overt expletive (e.g. Italian è estate)</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using different speech role designating items (if possible).
 For each example, provide one instance of a referentially indepentent pronoun (Mary likes him) and one instance where the same pronoun occurs as a variable bound by a quantified antecedent (everybody/no-one(i) believes that Mary likes him(i)).</t>
   </si>
@@ -4377,13 +4362,6 @@
   <si>
     <t>Provide at least two examples, using different speech role designating items.
 For each example, provide one instance where an adjective occurrs to the left of the head noun, and one instance where the same adjective occurs to the right of a speech role designating item.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no speech role designating items
-- Speech role designating items occur to the right of Adjectives/Numerals
-- The language has no prenominal Adjectives/Numerals
-If you want to provide any relevant example, do so in the Comments box</t>
   </si>
   <si>
     <t>This question can be answered only if the language has no article. If the language has an article, select the answer NO.</t>
@@ -4393,13 +4371,6 @@
 For each example, provide: 
 (1) one instance of a nominal argument where the cardinal numeral follows a possessive (or an adjective meaning 'other', 'same/even' or 'unique', or the noun itself) and the whole structure is interpreted as definite; 
 (2) one instance of a nominal argument where the same cardinal numeral precedes the same item(s) and the whole structure is not interepreted as definite.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has articles
-- the order of cardinal numerals and possessives/adjectives meaning 'other', 'same/even' or 'unique'/the noun itself is fixed
-- word order alternations of cardinal numerals and possessives/adjectives meaning 'other', 'same/even' or 'unique'/the noun itself are not associated with differences in the definite/non definite intepretation of the nominal argument
-If you want to provide any example, do so in the Comments box</t>
   </si>
   <si>
     <t>Provide at least two examples, with two different nouns. For each example, provide:
@@ -4437,18 +4408,6 @@
 For each adjective, provide two instances of different forms depending on different number interpretations of the head noun.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no group markers
-- The language has a group marker, but the latter does not occur on adjectives
-If you want to provide any relevant example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no group markers
-- The language has a group marker, but the latter does not occur twice in this type of sentences
-If you want to provide any relevant example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>If you answered YES to FGN_Qa, write "same examples as FGN_Qa".</t>
   </si>
   <si>
@@ -4469,22 +4428,8 @@
 For each adjective, provide two instances of different forms depending on different gender information encoded on the head noun.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- nominal arguments cannot be realized as bare
-- singular count nouns in argument position cannot be realized as bare
-- there are no singular vs. non-singular alternations on nouns
-- bare singular count nouns occurring in the object position of an atelic predicate never have number-neutral reading 
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using two different nouns.
 For each noun, provide one instance of it occurring bare in subject position with definite reading, and one instance of it occurring in subject position with a dedicated morpheme encoding indefinite/non presuppositional reading.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- there is no formal distinction between a noun with definite interpretation and a noun with no definite interpretation
-- there are systematic singular vs. non-singular alternations on nouns
-If you want to provide any example, do so in the Comments box</t>
   </si>
   <si>
     <t>Provide at least two examples, using two different nominal arguments.
@@ -4502,12 +4447,6 @@
   <si>
     <t>Provide at least two examples, using two different nominal arguments containing a plural and a mass noun, respectively.
 For each example, provide one instance where the noun is unambiguously interpreted as kind-referring (e.g. it is the subject of a predicate like be extinct/be introduced, or the object of a predicate like discover/create/invent) and is overtly marked, and one instance where the same noun is indefinite and has a different marker (or no marker at all).</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- nominal arguments cannot be realized as bare
-- singular count nouns in argument position cannot be realized as bare
-If you want to provide any example, do so in the Comments box</t>
   </si>
   <si>
     <t>To answer this question, follow the steps below:
@@ -4516,31 +4455,10 @@
 (3) If yes, can such a bare nominal argument have a definite interpretation?</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- the language has no non-adpositional Genitives
-- non adpositional Genitives only occur at the boundary of nominal structures
-- nouns cannot be bare when modified by (non adpositional) Genitives not occurring at the boundary of an argument nominal structure
-- bare nouns modified by a Genitive not occurring at the boundary do not have a definite interpretation
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using different nouns and demonstratives, if possible.
 For each example, provide one instance of a nominal argument containing a noun and an article, and one instance of a nominal argument where a demonstrative occurs with no article, in a position different than the position of the article.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- demonstratives systematically co-occur with articles
-- demonstratives are in complementary distribution with articles and systematically occur in the same position as articles
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no definiteness affixes
-- when a definite affix is attached to the noun, the latter occurs at the boundary of the nominal structure
-- when a definite affix is attached to the noun and the latter occurs in a non-boundary position, another overt definite category must appear at the boundary
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>This question can only be tested using an adjective that can occur in prenominal position only. If the language does not have such adjectives, select the answer NO.
 The question is relevant only in D-initial languages. If the language is D-final, select the answer NO.</t>
   </si>
@@ -4549,99 +4467,29 @@
 For each example, provide one instance of a nominal argument with an adjective modifying a common noun and occurring in prenominal position, and one instance of a bare nominal argument with the same adjective modifying a proper name and occurring in prenominal position.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- there are no prenominal adjectives
-- the language is D-final
-- all proper names systematically occur with an article in argument position (there are no bare argument proper names)
-- adjectives occur postnominally when modifying a bare proper name
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- there are no bare argument nouns
-- argument nominals with kind-referring interpretation always have an article
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- there are no bare nouns in subject position
-- argument nominals in subject position with generic interpretation always have an article
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Do not use a kinship noun in the singular to answer this question.</t>
   </si>
   <si>
     <t>For each example you provide, specify whether the definite intepretation is the only possible one by providing the relevant context (see DGR_Qa) or the ungrammatical/impossible interpretation.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- the language has no prenominal non-adpositional Genitives
-- when modified by a prenominal (non-adpositional) Genitives, the head noun agrees in phi-features with it
-- specific nominal arguments containing a prenominal Genitive cannot be bare
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>The question is relevant only in D-initial languages. If the language is D-final, select the answer NO.</t>
   </si>
   <si>
     <t>If you answered YES to CGR_Qd, and the examples you provided are relevant for this question as well, write "same examples as CGR_Qd"</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- the language has no definteness affixes
-- definite affixes only attach to initial constituents
-- the language is D-final</t>
-  </si>
-  <si>
     <t>This question can only be tested in languages that have possessives realized as independent lexical items that do not have to attach to any (nominal-like) head in pronominal function. If the language has no such items, the answer is NO.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no possessive items
-- the language has clitic possessives only
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one the following boxes:
-- the language has no subject-verb agreement
-- nominals unmarked as 1st/2nd person cannot control 1st/2nd verb agreement
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one the following boxes:
-- the language has no subject-verb agreement
-- there are no resumptive pronouns
-- 1st/2nd person pronouns cannot resume nominals unmarked as 1st/2nd person
-If you want to provide any example, do so in the Comments box</t>
   </si>
   <si>
     <t>Provide at least two examples. 
 For each example, provide one instance where the nominal argument has an article denoting non-proximity (in time or space), and one instance where the same noun is marked by an article denoting proximity (in time or space).</t>
   </si>
   <si>
-    <t>Check one the following boxes:
-- the language has no articles
-- articles encode no proximate vs. non-proximate distinction
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one the following boxes:
-- the language has no articles
-- articles encode no proximate vs. non-proximate distinction</t>
-  </si>
-  <si>
     <t>Provide examples using at least two different nouns.
 For each noun, provide at least one alternation in morphological Case/adposition such that one such Case/adposition assigns a partitive indefinite meaning while the other does not.</t>
   </si>
   <si>
-    <t>Check one of the following boxes.
-- the language has no Case morphology on nouns
-- partitive indefinite meaning is not expressed through adpositional alternations on bare head nouns
-- the language has Case morphology on nouns, but there are no morphological Case distinctions expressing partitive indefinite meaning as opposed to other readings
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Definite affixes are not to be analysed as part of the morphological make-up of a noun.</t>
   </si>
   <si>
@@ -4649,23 +4497,10 @@
 For each noun, provide one instance in which an article is suffixed to a noun modified by a postnominal modifier, and there is no other marker of the definite reading of the nominal structure.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- the language has no suffixed articles
-- the suffixed article is not the only marker of the definite reading of the nominal structure
-- the (suffixed) article is systematically phrase-final
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using different attributive adjectives.
 For each adjective, provide one instance in which an article is suffixed to the adjective, the latter is not the final item of the nominal structure and there is no other marker of the definite reading of the nominal structure.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- the language has no articles
-- articles cannot appear in nominal arguments that contain no overt noun
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using different nouns.
 For each noun, provide two instances: one with a definite determiner and one where no definite determiner appears and the noun (and possibly the adjective) has a special marker that only appears in the absence of the definite determiner.</t>
   </si>
@@ -4676,12 +4511,6 @@
     <t>You can use the same contexts as those of DGR_Qb.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- the language has no classifier
-- bare nominals without an overt classifier can receive a definite specific interpretation
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using different nouns.
 For each noun, provide instances with at least three different persons, if possible.</t>
   </si>
@@ -4690,59 +4519,20 @@
 For each adjective, provide one instance of an indefinite argument in which the adjective appears to the left of a cardinal numeral and one instance in which the adjective appears to the right of the same cardinal numeral.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no postnominal arguments
-- The language has postnominal arguments but adjectives do not follow them
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no prenominal Argument adjectives
-- The language has prenominal Argument adjectives but no postnominal adjectives
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using different nouns.
 For each noun, provide one instance where the noun is not modified by a Genitive and one where it is modified by a Genitive and has a different morpho-phonological form.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitive arguments
-- The form of the noun does not change depending on whether it is modified by a non-adpositional Genitive argument or not
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using different nouns modified by a Genitive argument.
 For each noun, provide one instance where the noun is modified by a 3rd person Genitive argument and one instance where it is modified by a 1st or 2nd person Genitive argument and has a different morpho-phonological form.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The form of the noun does not change depending on whether it is modified by a Genitive or not
-- The form of the noun does not change depending on whether it is modified by a 3rd person Genitive or not
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using different nouns modified by a Genitive argument.
 For each noun, provide one instance where the noun is modified by a 1st person Genitive argument and one instance where it is modified by a 2nd person Genitive argument and has a different morpho-phonological form.</t>
   </si>
   <si>
-    <t>Check one of the following boxes.
-- The language has no non-adpositional Genitives
-- The form of the noun does not change depending on whether it is modified by a Genitive or not
-- The form of the noun does not change depending on whether it is modified by a 1st or 2nd person Genitive
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using different nouns modified by a Genitive/possessive argument.
 For each noun, provide one instance where the noun is modified by a 3rd person Genitive argument and one instance where it is modified by a 1st or 2nd person Genitive argument and has a different morpho-phonological form.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The form of the noun does not change depending on whether it is modified by a Genitive or not
-- The form of the noun does not change depending on whether it is modified by a 3rd or by a 1st/2nd person Genitive
-If you want to provide any example, do so in the Comments box.</t>
   </si>
   <si>
     <t>This question applies to languages that have nominative/accusative alignment in clauses.
@@ -4752,13 +4542,6 @@
 The answer is YES if the internal argument of the noun bears the same case morphology (or the same special marking) as the internal argument of the verb, different from that found on the external argument.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no nominative/accusative alignment in clauses
-- The language has no special marking for the internal argument of the verb
-- The internal argument of the noun does not bear the same case morphology/special marking as the internal argument of the verb
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>To answer this question, look for the following evidence:
 (1) a nominal structure whose head noun is modified by an oblique argument;
 (2) a sentence where the verb is modified by the same type of oblique argument.
@@ -4770,64 +4553,6 @@
 For each example, provide an instance of a nominal argument where the noun is modified by an oblique argument, and an instance of a verb modified by an oblique complement that is introduced by the same morpheme as the complement of the noun.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no definiteness suffixes
-- Nouns/Adjectives bearing a definiteness suffix cannot be immediately followed by a possessive
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no definiteness suffixes
-- Nouns or adjectives bearing a definiteness suffix are not followed by a full genitive phrase whose determiner position hosts a Genitive-marked element
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitive arguments
-- The language has no systematic morpho-phonological affixation on head nouns depending on the presence of a non-adpositional genitive argument
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The language has no non-adpositional prenominal Genitives
-- The language has no non-adpositional postnominal Genitives
-- The language has no prenominal Adjectives
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The language has no non-adpositional prenominal Genitives
-- The language has no non-adpositional postnominal Genitives
-- Only one non-adpositional Genitive can be realized in prenominal position
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The language has no non-adpositional postnominal Genitives
-- The language has no postnominal adjectives
-- Only one non-adpositional Genitive is allowed in postnominal position
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The language has no prenominal non-adpositional Genitives
-- The language has no non-adpositional postnominal Genitives
-- Only one non-adpositional Genitive can be realized in prenominal position
-- The language has no prenominal Adjectives
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>SOTTO NO
-Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The language does not allow more than two occurrences of non-adpositional Genitives
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>Do not use a pronominal possessive to answer this question.</t>
   </si>
   <si>
@@ -4835,40 +4560,7 @@
 If your answer to ARR_Qb is YES, to answer the present question you must provide evidence of an adjective that follows a numeral in an indefinite nominal argument, and precedes a non-adpositional genitive functioning as an argument or alienable possessor of the noun.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The language has no non-adpositional Genitives functioning as arguments or alienable possessors of the noun
-- Adjectives do not precede non-adpositional Genitives
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>Do not use nominals with 'home' as a head noun to answer this question.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The language has no non-adpositional Genitives functioning as arguments or alienable possessors of the noun
-- The language has no non-adpositional Genitives following the head noun
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- Adjectives do not precede non-adpositional Genitives
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The language has no non-adpositional Genitives following the head noun
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The language has no prenominal Adjectives
-- Genitives realized as a visibly branching phrase headed by a common noun do not precede prenominal adjectives
-If you want to provide any example, do so in the Comments box.</t>
   </si>
   <si>
     <t>To answer this question, look for two nominal arguments headed by the following nouns:
@@ -4876,12 +4568,6 @@
 (2) one noun denoting an entity that is not inalienably possessed (e.g. dog, house, ...: 'I saw an ugly house/dog').
 The answer is YES if, when these nouns are realized without a visible possessor, a morpheme agreeing with the arbitrary possessor appear on the inalienably possessed noun but not on the other one.
 The answer is NO if the noun has the same morphological make up in both cases.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no non-adpositional Genitives
-- The language does not resort to an additional nominal head to license a second genitive argument
-If you want to provide any example, do so in the Comments box.</t>
   </si>
   <si>
     <t xml:space="preserve">Test this question with different types of cardinal expressions, for example:
@@ -4892,20 +4578,8 @@
 </t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- Cardinal expressions do not inflect for gender
-- The language exhibit no agreement in gender within nominal structures
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>Provide at least two examples of indefinite nominal arguments, with different nouns and cardinal expressions.
 For each noun, provide one instance where it is modified by a cardinal expression higher than 'two' and is marked plural, and one instance where it has singular interpretation and is marked differently (or unmarked).</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no Number morphology
-- The noun does not bear plural marking when occcurring with a cardinal
-If you want to provide any example, do so in the Comments box.</t>
   </si>
   <si>
     <t>To answer this question, look for a nominal structure where the cardinal expression modifies a noun, and provide two instances of it: 
@@ -4914,24 +4588,12 @@
 The answer is YES if the noun bears overt plural marking only when the definite determiner is overt.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no overt number morphology
-- The noun bears no overt plural marking when a definite determiner cooccurs with a non-compound cardinal numeral higher than ‘two’
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>To answer this question, look for a nominal structure where the cardinal expression modifies a noun, and provide two instances of it: 
 (1) one instance where the noun is interpreted as definite;
 (2) one instance where the noun is interpreted as non definite.
 The answer is YES if the noun bears overt plural marking only when it is interpreted as definite.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no overt number morphology
-- The noun bears no overt plural marking when modified by a non-compound cardinal numeral higher than ‘two’
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>Provide at least two examples, using different numerals.
 For each example, provide at least two instances, one where the numeral is realized as "personal", the other where it does not appear with any personal morpheme.</t>
   </si>
@@ -4948,84 +4610,10 @@
 For each example, provide two instances, one where the verb is found in a main clause whose subject is overt and marked as such, the other where the same verb is found in a relative clause whose subject is overt, is different from the noun heading the relative clause and is assigned a case that is different from the first example.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no morphological case distinctions
-- The language has no cases that are exclusively adnominal
-- Overt transitive subjects of relative clauses are assigned the same case as overt transitive subjects of main clauses
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- there is no definiteness marker on nouns
-- relative clauses headed by nouns marked as definite are not different from those headed by nouns not marked as definite 
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>Provide at least two instances of one and the same adposition/linker displaying morphological alternations controlled by phi-features of the head noun.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- the language has no adpositional Genitives/linkers
-- the morphological form of adpositions/linkers does not display any alternations controlled by phi-features of the head noun
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
     <t>To test this question, use nouns like: present/gift; letter; photo; trip.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no adpositions
-- adpositions follow their complements (i.e. are realized as postpositions)
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no adpositional Genitives
-- adpositional Genitives precede their complements
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no linkers
-- linkers follow their complements
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no linkers
-- linker prases precede their head nouns
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no adpositions
-- adpositions precede their complements (i.e. are realized as prepositions)
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no adpositional Genitives
-- adpositional Genitives follow their complements
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no articles
-- the article occurs as the last word and is preceded by some other overt element belonging to the nominal phrase
-- the article occurs affixed to the last word, and is preceded by some other overt element belonging to the nominal phrase
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- there are no positional alternations affecting cardinals/numerical adjectives and Genitives or possessives
-- positional alternations affecting cardinals/numerical adjectives and Genitives or possessives are not associated with different interpretations (e.g., definite vs. indefinite reading)
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no articles
-- the article occurs as the first word or affixed to the first word, and is followed by some other overt element belonging to the nominal phrase
-If you want to provide any example, do so in the Comments box.</t>
   </si>
   <si>
     <t>Do not use the cardinal for 'one' to test this question.
@@ -5044,48 +4632,14 @@
     <t>If you answered YES to NM1_Qa, write "same examples as NM1_Qa".</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- the language has no non-adpositional Genitives
-- the language has no non-adpositional prenominal Genitives
-- the language has no prenominal adjectives
-- non-adpositional Genitives never occurr between a structured adjective and a noun
-If you want to provide any example, do so in the Comments box.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no non-adpositional Genitives
-- the language has no postnominal adjectives
-- the language has no postnominal adjectives occurring to the left of non-adpositional Genitives
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- the language has no postnominal adjectives
-- the language has no adjectives alternating between the pre- and post-nominal position
-- there are no interpretive alternations between pre- and postnominal position
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Provide at least two examples of a definite nominal argument modified by an adjective, using different nouns/adjectives.
 For each example, provide two instances: one where the noun occurs with no modifiers and has a definiteness suffix, one where the same noun is modified by an adjective and has a definite suffix, and a non-suffixal article appears as well.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- the language has no definiteness suffixes
-- if a definite suffix occurs on the noun (or on any other modifier) no non-suffixal articles appear
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Provide at least two examples of a definite nominal argument, using different nouns.
 For each example, provide two instances: one where the noun occurs with no modifiers and has a definiteness suffix, one where the nominal argument has a demontrative at the boundary and the noun has a definite suffix.</t>
   </si>
   <si>
-    <t>Check one of the following boxes
-- the language has no definiteness suffixes
-- if a demonstrative appears at the boundary, no definite suffix is visible on the noun
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>To answer this question, use/adapt the evidence collected to answer the questions of parameter ARR. 
 If no questions for parameter ARR has a YES, the answer to this question is NO.</t>
   </si>
@@ -5093,12 +4647,6 @@
     <t>If you provided examples with definite nominal structures to answer the questions of parameter ARR, write "same examples as ARR".</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- the language has no adjectives realized as reduced relative clauses
-- no article appears before adjectives realized as reduced relative clauses in definite nominal arguments
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>If the language has multiple positions for adjectival modifiers, test this question with all possible positions.
 To answer YES, it is sufficient that the definite article is systematically replicated at least in one position.</t>
   </si>
@@ -5107,13 +4655,6 @@
 To answer YES, it is necessary for the definite article not to be duplicated on any adjectival position.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no prenominal cardinal numerals
-- The language has no definiteness suffixes
-- Definiteness suffixes are never found on cardinal numerals
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Test this question with various classes of proper names (e.g., names of individuals, cities, regions, islands, states, rivers, etc.).
 The answer is YES if at least one such class of names can appear without an article when used as an argument.</t>
   </si>
@@ -5129,22 +4670,7 @@
 This question can be tested only in languages where non-adpositional genitives do not occur to the left of the noun and after adjectives: if your answer to NGL_Qa is YES, then your answer to the present question must be NO.</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has non-adpositional genitives occurring between an adjective/numeral and the noun
-- The language has no non-adpositional genitives
-- The language has no prenominal adjectives/numerals
-- Possessives are never realized after a prenominal adjectives
-- Possessives can be realized after a prenominal adjective, but are not uninflected
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>This question can be tested only in languages with linkers: if your answers to LKO_Qa and LKP_Qa are both NO, then your answer to the present question must be NO as well.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes
-- The language has no linkers
-- Possessives are never realized as clitics directly attached to the noun
-If you want to provide any example, do so in the Comments box</t>
   </si>
   <si>
     <t>This question can be tested only in languages where adjectives can be postnominal. If your language has no postnominal adjectives, the answer to the present question is NO.
@@ -5152,12 +4678,6 @@
   </si>
   <si>
     <t>Provide at least two examples, using different nouns and adjectives. For each example, provide one instance where the head noun is modified by a postnominal adjective and one instance where the same head noun, in the same context, is modified by a possessive occurring in the same postnominal position as the adjective.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no postnominal adjectives
-- The language has no postnominal possessives occurringwith the same distribution as postnominal adjectives
-If you want to provide any example, do so in the Comments box</t>
   </si>
   <si>
     <t>This question can be tested only in languages where adjectives can be prenominal as a general rule. If your language has no prenominal adjectives (i.e., if your answer to NM1_Qa is NO), the answer to the present question is NO.
@@ -5168,12 +4688,6 @@
     <t>Provide at least two examples, using different nouns and adjectives. For each example, provide one instance where the head noun is modified by a numeral followed by a prenominal adjective and one instance where the same head noun, in the same context, is modified by a possessive occurring in the same position as the adjective (i.e., after the numeral and before the noun).</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- The language has no prenominal adjectives
-- The language has no prenominal possessives occurring with the same distribution as prenominal adjectives
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>Test this question with argument adjectives from personal proper names and common nouns.</t>
   </si>
   <si>
@@ -5198,12 +4712,6 @@
   <si>
     <t>Provide at least two examples, using different nouns. 
 For each example, provide one instance where the head noun is modified by a postnominal adjective and one where the same head noun, in the same context, is modified by a demonstrative occurring in the same position as the adjective.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no postnominal adjectives
-- The language has no postnominal demonstratives occurring with the same distribution as postnominal adjectives
-If you want to provide any example, do so in the Comments box</t>
   </si>
   <si>
     <t>This question can be tested only in languages where adjectives can be fronted to the left of determiners/numerals. If adjectives cannot be fronted in your language, the answer to the present question is NO.</t>
@@ -5216,67 +4724,7 @@
 (4) the demonstrative is fronted to the same position as the adjective in (2).</t>
   </si>
   <si>
-    <t>Check one of the following boxes:
-- Adjectives cannot be fronted
-- Demonstratives cannot occur in the same position as fronted adjectives
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- The language has no definiteness affixes
-- Demonstratives are not found after a noun bearing a definiteness affix
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- Demonstratives are split
-- Demonstratives and adjectives cannot be freely ordered
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
     <t>This question does not apply to split Demonstratives: the answer is NO if you answered YES to TSP_Qa or TSP_Qb.</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- Demonstratives are split
-- Demonstratives and adpositional genitives cannot be freely ordered
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- Demonstratives are split
-- Demonstratives and relative clauses cannot be freely ordered
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- Demonstratives are split
-- Demonstratives and the numeral 'one' cannot be freely ordered
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- Demonstratives are split
-- Demonstratives and numerals cannot be freely ordered
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- Demonstratives are split
-- Demonstratives and PPs cannot be freely ordered
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- Demonstratives are split
-- The language has no determinerless nominal arguments headed by a singular count noun
-If you want to provide any example, do so in the Comments box</t>
-  </si>
-  <si>
-    <t>Check one of the following boxes:
-- Demonstratives do not cooccur with articles
-- No copy of the definite article introducing the noun occurs on demonstratives
-If you want to provide any example, do so in the Comments box</t>
   </si>
   <si>
     <t>This question does not apply to adjectival demonstratives: if your answer to TSA_Qb is YES, the answer to the present question must be NO.
@@ -5557,6 +5005,33 @@
   </si>
   <si>
     <t>FGN_Qc</t>
+  </si>
+  <si>
+    <t>Check one of the following boxes. If you want to provide any example, do so in the Comments box</t>
+  </si>
+  <si>
+    <t>Provide an example with no overt expletive (e.g. Italian 'È estate')</t>
+  </si>
+  <si>
+    <t>Check one of the following boxes.
+If you want to provide any relevant example, do so in the Comments box</t>
+  </si>
+  <si>
+    <t>Check one of the following boxes. If you want to provide any relevant example, do so in the Comments box</t>
+  </si>
+  <si>
+    <t>Check one the following boxes. If you want to provide any example, do so in the Comments box</t>
+  </si>
+  <si>
+    <t>Check one of the following boxes. If you want to provide any example, do so in the Comments box.</t>
+  </si>
+  <si>
+    <t>Check one of the following boxes.
+If you want to provide any example, do so in the Comments box.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Check one of the following boxes. If you want to provide any example, do so in the Comments box.</t>
   </si>
 </sst>
 </file>
@@ -6005,16 +5480,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF7F8A9-63CE-4FE3-9607-7AA57A6C5082}">
   <dimension ref="A1:I255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" topLeftCell="A255" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A235" sqref="A235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="109.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="82.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
     <col min="5" max="7" width="29" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5" style="1" bestFit="1" customWidth="1"/>
@@ -6038,7 +5514,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1040</v>
+        <v>954</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>613</v>
@@ -6127,7 +5603,7 @@
         <v>846</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>847</v>
+        <v>981</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
@@ -6147,7 +5623,7 @@
         <v>621</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
@@ -6167,7 +5643,7 @@
         <v>622</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -6190,7 +5666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="176" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="160" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -6204,10 +5680,10 @@
         <v>826</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>851</v>
+        <v>981</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
@@ -6227,7 +5703,7 @@
         <v>827</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="I10" s="1">
         <v>1</v>
@@ -6247,7 +5723,7 @@
         <v>828</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
@@ -6284,10 +5760,10 @@
         <v>624</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>855</v>
+        <v>982</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
@@ -6324,13 +5800,13 @@
         <v>626</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="176" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -6344,19 +5820,19 @@
         <v>829</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>859</v>
+        <v>983</v>
       </c>
       <c r="I16" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="256" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="240" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -6370,13 +5846,13 @@
         <v>627</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>862</v>
+        <v>981</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
@@ -6413,7 +5889,7 @@
         <v>789</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
@@ -6433,10 +5909,10 @@
         <v>629</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>865</v>
+        <v>860</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
@@ -6456,7 +5932,7 @@
         <v>790</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>866</v>
+        <v>861</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -6527,7 +6003,7 @@
         <v>832</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -6535,7 +6011,7 @@
     </row>
     <row r="26" spans="1:9" ht="224" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>1065</v>
+        <v>979</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>104</v>
@@ -6547,7 +6023,7 @@
         <v>633</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>868</v>
+        <v>863</v>
       </c>
       <c r="I26" s="1">
         <v>0</v>
@@ -6555,7 +6031,7 @@
     </row>
     <row r="27" spans="1:9" ht="224" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>1066</v>
+        <v>980</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>104</v>
@@ -6567,7 +6043,7 @@
         <v>791</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>869</v>
+        <v>864</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -6607,7 +6083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -6621,7 +6097,7 @@
         <v>636</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>870</v>
+        <v>983</v>
       </c>
       <c r="I30" s="1">
         <v>0</v>
@@ -6644,7 +6120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -6658,7 +6134,7 @@
         <v>833</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>871</v>
+        <v>984</v>
       </c>
       <c r="I32" s="1">
         <v>0</v>
@@ -6695,7 +6171,7 @@
         <v>832</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>872</v>
+        <v>865</v>
       </c>
       <c r="I34" s="1">
         <v>0</v>
@@ -6715,7 +6191,7 @@
         <v>638</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>873</v>
+        <v>866</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
@@ -6769,7 +6245,7 @@
         <v>640</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>874</v>
+        <v>867</v>
       </c>
       <c r="I38" s="1">
         <v>0</v>
@@ -6857,7 +6333,7 @@
         <v>644</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>875</v>
+        <v>868</v>
       </c>
       <c r="I43" s="1">
         <v>0</v>
@@ -6914,7 +6390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="288" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
@@ -6928,13 +6404,13 @@
         <v>648</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>876</v>
+        <v>981</v>
       </c>
       <c r="I47" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="288" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
@@ -6948,10 +6424,10 @@
         <v>649</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>878</v>
+        <v>981</v>
       </c>
       <c r="I48" s="1">
         <v>0</v>
@@ -7005,7 +6481,7 @@
         <v>793</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>879</v>
+        <v>870</v>
       </c>
       <c r="I51" s="1">
         <v>0</v>
@@ -7025,7 +6501,7 @@
         <v>794</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>880</v>
+        <v>871</v>
       </c>
       <c r="I52" s="1">
         <v>0</v>
@@ -7045,7 +6521,7 @@
         <v>795</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>881</v>
+        <v>872</v>
       </c>
       <c r="I53" s="1">
         <v>0</v>
@@ -7065,7 +6541,7 @@
         <v>796</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>882</v>
+        <v>873</v>
       </c>
       <c r="I54" s="1">
         <v>0</v>
@@ -7139,7 +6615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="160" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>48</v>
       </c>
@@ -7153,13 +6629,13 @@
         <v>655</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>883</v>
+        <v>981</v>
       </c>
       <c r="I59" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="256" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="304" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>49</v>
       </c>
@@ -7173,16 +6649,16 @@
         <v>656</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>884</v>
+        <v>874</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>885</v>
+        <v>981</v>
       </c>
       <c r="I60" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="176" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="192" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>50</v>
       </c>
@@ -7196,16 +6672,16 @@
         <v>657</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>886</v>
+        <v>875</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>887</v>
+        <v>981</v>
       </c>
       <c r="I61" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="208" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>51</v>
       </c>
@@ -7219,7 +6695,7 @@
         <v>658</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>888</v>
+        <v>981</v>
       </c>
       <c r="I62" s="1">
         <v>0</v>
@@ -7239,13 +6715,13 @@
         <v>659</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>889</v>
+        <v>876</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>890</v>
+        <v>877</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>891</v>
+        <v>981</v>
       </c>
       <c r="I63" s="1">
         <v>0</v>
@@ -7265,10 +6741,10 @@
         <v>660</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>1033</v>
+        <v>947</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>892</v>
+        <v>981</v>
       </c>
       <c r="I64" s="1">
         <v>0</v>
@@ -7291,7 +6767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>54</v>
       </c>
@@ -7305,16 +6781,16 @@
         <v>662</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>1034</v>
+        <v>948</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>893</v>
+        <v>981</v>
       </c>
       <c r="I66" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="192" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>55</v>
       </c>
@@ -7328,19 +6804,19 @@
         <v>663</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>894</v>
+        <v>878</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>895</v>
+        <v>879</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>896</v>
+        <v>981</v>
       </c>
       <c r="I67" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="192" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>56</v>
       </c>
@@ -7354,13 +6830,13 @@
         <v>664</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>897</v>
+        <v>880</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>898</v>
+        <v>881</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>899</v>
+        <v>981</v>
       </c>
       <c r="I68" s="1">
         <v>0</v>
@@ -7380,16 +6856,16 @@
         <v>665</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>900</v>
+        <v>882</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>901</v>
+        <v>981</v>
       </c>
       <c r="I69" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="320" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>58</v>
       </c>
@@ -7403,13 +6879,13 @@
         <v>666</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>902</v>
+        <v>985</v>
       </c>
       <c r="I70" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="395" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>59</v>
       </c>
@@ -7423,13 +6899,13 @@
         <v>667</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>903</v>
+        <v>985</v>
       </c>
       <c r="I71" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="240" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>60</v>
       </c>
@@ -7443,16 +6919,16 @@
         <v>668</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>904</v>
+        <v>883</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>905</v>
+        <v>985</v>
       </c>
       <c r="I72" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>532</v>
       </c>
@@ -7466,13 +6942,13 @@
         <v>669</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>906</v>
+        <v>985</v>
       </c>
       <c r="I73" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="240" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>61</v>
       </c>
@@ -7486,10 +6962,10 @@
         <v>798</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>907</v>
+        <v>884</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>908</v>
+        <v>981</v>
       </c>
       <c r="I74" s="1">
         <v>0</v>
@@ -7509,13 +6985,13 @@
         <v>670</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>909</v>
+        <v>885</v>
       </c>
       <c r="I75" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="128" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>62</v>
       </c>
@@ -7529,16 +7005,16 @@
         <v>836</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>910</v>
+        <v>886</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>911</v>
+        <v>981</v>
       </c>
       <c r="I76" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="176" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>63</v>
       </c>
@@ -7552,16 +7028,16 @@
         <v>671</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>912</v>
+        <v>887</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>911</v>
+        <v>981</v>
       </c>
       <c r="I77" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>64</v>
       </c>
@@ -7575,13 +7051,13 @@
         <v>672</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>913</v>
+        <v>981</v>
       </c>
       <c r="I78" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="350" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>65</v>
       </c>
@@ -7595,13 +7071,13 @@
         <v>673</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>913</v>
+        <v>981</v>
       </c>
       <c r="I79" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="224" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>66</v>
       </c>
@@ -7615,7 +7091,7 @@
         <v>674</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>913</v>
+        <v>981</v>
       </c>
       <c r="I80" s="1">
         <v>0</v>
@@ -7635,7 +7111,7 @@
         <v>837</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>914</v>
+        <v>888</v>
       </c>
       <c r="I81" s="1">
         <v>0</v>
@@ -7689,13 +7165,13 @@
         <v>614</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>915</v>
+        <v>889</v>
       </c>
       <c r="I84" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="208" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>69</v>
       </c>
@@ -7709,10 +7185,10 @@
         <v>677</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>916</v>
+        <v>890</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>917</v>
+        <v>981</v>
       </c>
       <c r="I85" s="1">
         <v>0</v>
@@ -7749,7 +7225,7 @@
         <v>679</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>918</v>
+        <v>891</v>
       </c>
       <c r="I87" s="1">
         <v>0</v>
@@ -7769,7 +7245,7 @@
         <v>799</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>918</v>
+        <v>891</v>
       </c>
       <c r="I88" s="1">
         <v>1</v>
@@ -7840,13 +7316,13 @@
         <v>681</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>919</v>
+        <v>892</v>
       </c>
       <c r="I92" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="208" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>74</v>
       </c>
@@ -7860,13 +7336,13 @@
         <v>682</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>920</v>
+        <v>986</v>
       </c>
       <c r="I93" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>75</v>
       </c>
@@ -7880,13 +7356,13 @@
         <v>683</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>921</v>
+        <v>986</v>
       </c>
       <c r="I94" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="224" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="256" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>76</v>
       </c>
@@ -7900,10 +7376,10 @@
         <v>684</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>922</v>
+        <v>893</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>923</v>
+        <v>986</v>
       </c>
       <c r="I95" s="1">
         <v>0</v>
@@ -7926,7 +7402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="192" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="176" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>77</v>
       </c>
@@ -7940,10 +7416,10 @@
         <v>686</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>924</v>
+        <v>894</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>925</v>
+        <v>986</v>
       </c>
       <c r="I97" s="1">
         <v>0</v>
@@ -7966,7 +7442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="192" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="224" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>78</v>
       </c>
@@ -7980,10 +7456,10 @@
         <v>688</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>926</v>
+        <v>895</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>927</v>
+        <v>986</v>
       </c>
       <c r="I99" s="1">
         <v>0</v>
@@ -8006,7 +7482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="240" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" ht="350" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>79</v>
       </c>
@@ -8020,10 +7496,10 @@
         <v>689</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>928</v>
+        <v>896</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>929</v>
+        <v>986</v>
       </c>
       <c r="I101" s="1">
         <v>0</v>
@@ -8111,10 +7587,10 @@
         <v>803</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>930</v>
+        <v>897</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>931</v>
+        <v>986</v>
       </c>
       <c r="I106" s="1">
         <v>0</v>
@@ -8168,7 +7644,7 @@
         <v>804</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>932</v>
+        <v>898</v>
       </c>
       <c r="I109" s="1">
         <v>0</v>
@@ -8188,7 +7664,7 @@
         <v>694</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>933</v>
+        <v>899</v>
       </c>
       <c r="I110" s="1">
         <v>1</v>
@@ -8245,7 +7721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="192" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="224" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>88</v>
       </c>
@@ -8259,13 +7735,13 @@
         <v>698</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>934</v>
+        <v>986</v>
       </c>
       <c r="I114" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" ht="208" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>89</v>
       </c>
@@ -8279,13 +7755,13 @@
         <v>699</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>935</v>
+        <v>986</v>
       </c>
       <c r="I115" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="256" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>90</v>
       </c>
@@ -8299,13 +7775,13 @@
         <v>838</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>936</v>
+        <v>986</v>
       </c>
       <c r="I116" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="176" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>91</v>
       </c>
@@ -8319,13 +7795,13 @@
         <v>805</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>937</v>
+        <v>986</v>
       </c>
       <c r="I117" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="192" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" ht="365" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>92</v>
       </c>
@@ -8339,13 +7815,13 @@
         <v>700</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>938</v>
+        <v>986</v>
       </c>
       <c r="I118" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="192" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" ht="350" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>93</v>
       </c>
@@ -8359,7 +7835,7 @@
         <v>701</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>939</v>
+        <v>987</v>
       </c>
       <c r="I119" s="1">
         <v>0</v>
@@ -8379,13 +7855,13 @@
         <v>806</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>940</v>
+        <v>986</v>
       </c>
       <c r="I120" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>95</v>
       </c>
@@ -8399,7 +7875,7 @@
         <v>807</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>941</v>
+        <v>988</v>
       </c>
       <c r="I121" s="1">
         <v>0</v>
@@ -8436,7 +7912,7 @@
         <v>702</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>942</v>
+        <v>900</v>
       </c>
       <c r="I123" s="1">
         <v>1</v>
@@ -8459,7 +7935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="240" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>97</v>
       </c>
@@ -8473,16 +7949,16 @@
         <v>703</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>943</v>
+        <v>901</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>944</v>
+        <v>986</v>
       </c>
       <c r="I125" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="288" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>98</v>
       </c>
@@ -8496,16 +7972,16 @@
         <v>704</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>945</v>
+        <v>902</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>946</v>
+        <v>986</v>
       </c>
       <c r="I126" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="208" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="395" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>99</v>
       </c>
@@ -8519,16 +7995,16 @@
         <v>705</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>1035</v>
+        <v>949</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>947</v>
+        <v>986</v>
       </c>
       <c r="I127" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" ht="304" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>100</v>
       </c>
@@ -8542,13 +8018,13 @@
         <v>706</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>948</v>
+        <v>986</v>
       </c>
       <c r="I128" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="176" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" ht="160" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>263</v>
       </c>
@@ -8562,7 +8038,7 @@
         <v>707</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>949</v>
+        <v>986</v>
       </c>
       <c r="I129" s="1">
         <v>0</v>
@@ -8633,7 +8109,7 @@
         <v>808</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>950</v>
+        <v>903</v>
       </c>
       <c r="I133" s="1">
         <v>0</v>
@@ -8670,7 +8146,7 @@
         <v>712</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>1036</v>
+        <v>950</v>
       </c>
       <c r="I135" s="1">
         <v>0</v>
@@ -8693,7 +8169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" ht="350" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>266</v>
       </c>
@@ -8707,7 +8183,7 @@
         <v>809</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>951</v>
+        <v>986</v>
       </c>
       <c r="I137" s="1">
         <v>0</v>
@@ -8747,7 +8223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" ht="288" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>268</v>
       </c>
@@ -8761,10 +8237,10 @@
         <v>810</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>952</v>
+        <v>904</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>953</v>
+        <v>986</v>
       </c>
       <c r="I140" s="1">
         <v>0</v>
@@ -8818,10 +8294,10 @@
         <v>717</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>954</v>
+        <v>905</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>955</v>
+        <v>986</v>
       </c>
       <c r="I143" s="1">
         <v>0</v>
@@ -8858,16 +8334,16 @@
         <v>812</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>956</v>
+        <v>906</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>957</v>
+        <v>986</v>
       </c>
       <c r="I145" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="192" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" ht="208" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>271</v>
       </c>
@@ -8881,10 +8357,10 @@
         <v>813</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>958</v>
+        <v>907</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>959</v>
+        <v>986</v>
       </c>
       <c r="I146" s="1">
         <v>0</v>
@@ -8924,7 +8400,7 @@
         <v>845</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>960</v>
+        <v>908</v>
       </c>
       <c r="I148" s="1">
         <v>0</v>
@@ -8964,7 +8440,7 @@
         <v>845</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>961</v>
+        <v>909</v>
       </c>
       <c r="I150" s="1">
         <v>0</v>
@@ -9001,7 +8477,7 @@
         <v>723</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>962</v>
+        <v>910</v>
       </c>
       <c r="I152" s="1">
         <v>0</v>
@@ -9024,7 +8500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>276</v>
       </c>
@@ -9038,16 +8514,16 @@
         <v>840</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>963</v>
+        <v>911</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>964</v>
+        <v>986</v>
       </c>
       <c r="I154" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="350" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>277</v>
       </c>
@@ -9061,10 +8537,10 @@
         <v>725</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>1037</v>
+        <v>951</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>965</v>
+        <v>986</v>
       </c>
       <c r="I155" s="1">
         <v>0</v>
@@ -9087,7 +8563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="288" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" ht="350" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>278</v>
       </c>
@@ -9101,10 +8577,10 @@
         <v>841</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>966</v>
+        <v>912</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>967</v>
+        <v>986</v>
       </c>
       <c r="I157" s="1">
         <v>0</v>
@@ -9141,7 +8617,7 @@
         <v>814</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>968</v>
+        <v>913</v>
       </c>
       <c r="I159" s="1">
         <v>0</v>
@@ -9161,13 +8637,13 @@
         <v>815</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>968</v>
+        <v>913</v>
       </c>
       <c r="I160" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>280</v>
       </c>
@@ -9181,13 +8657,13 @@
         <v>728</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>969</v>
+        <v>986</v>
       </c>
       <c r="I161" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>281</v>
       </c>
@@ -9201,13 +8677,13 @@
         <v>729</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>970</v>
+        <v>986</v>
       </c>
       <c r="I162" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" ht="128" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>282</v>
       </c>
@@ -9221,13 +8697,13 @@
         <v>730</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>971</v>
+        <v>986</v>
       </c>
       <c r="I163" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" ht="128" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>283</v>
       </c>
@@ -9241,13 +8717,13 @@
         <v>730</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>972</v>
+        <v>986</v>
       </c>
       <c r="I164" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="350" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>561</v>
       </c>
@@ -9261,13 +8737,13 @@
         <v>731</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>973</v>
+        <v>986</v>
       </c>
       <c r="I165" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>562</v>
       </c>
@@ -9281,13 +8757,13 @@
         <v>732</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>974</v>
+        <v>986</v>
       </c>
       <c r="I166" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="192" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" ht="208" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>284</v>
       </c>
@@ -9301,13 +8777,13 @@
         <v>733</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>975</v>
+        <v>986</v>
       </c>
       <c r="I167" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="208" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" ht="240" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>285</v>
       </c>
@@ -9321,13 +8797,13 @@
         <v>734</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>976</v>
+        <v>986</v>
       </c>
       <c r="I168" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" ht="272" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>571</v>
       </c>
@@ -9341,7 +8817,7 @@
         <v>816</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>977</v>
+        <v>986</v>
       </c>
       <c r="I169" s="1">
         <v>1</v>
@@ -9381,7 +8857,7 @@
         <v>735</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>978</v>
+        <v>914</v>
       </c>
       <c r="I171" s="1">
         <v>0</v>
@@ -9401,7 +8877,7 @@
         <v>736</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>978</v>
+        <v>914</v>
       </c>
       <c r="I172" s="1">
         <v>1</v>
@@ -9421,7 +8897,7 @@
         <v>737</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>979</v>
+        <v>915</v>
       </c>
       <c r="I173" s="1">
         <v>0</v>
@@ -9458,7 +8934,7 @@
         <v>739</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>980</v>
+        <v>916</v>
       </c>
       <c r="I175" s="1">
         <v>0</v>
@@ -9478,7 +8954,7 @@
         <v>740</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>981</v>
+        <v>917</v>
       </c>
       <c r="I176" s="1">
         <v>1</v>
@@ -9498,7 +8974,7 @@
         <v>741</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>982</v>
+        <v>918</v>
       </c>
       <c r="I177" s="1">
         <v>0</v>
@@ -9535,7 +9011,7 @@
         <v>740</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>981</v>
+        <v>917</v>
       </c>
       <c r="I179" s="1">
         <v>1</v>
@@ -9572,7 +9048,7 @@
         <v>740</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>981</v>
+        <v>917</v>
       </c>
       <c r="I181" s="1">
         <v>1</v>
@@ -9592,13 +9068,13 @@
         <v>616</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>981</v>
+        <v>917</v>
       </c>
       <c r="I182" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="224" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>293</v>
       </c>
@@ -9612,13 +9088,13 @@
         <v>744</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>983</v>
+        <v>986</v>
       </c>
       <c r="I183" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:9" ht="128" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>294</v>
       </c>
@@ -9635,13 +9111,13 @@
         <v>845</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="I184" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="176" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:9" ht="288" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>295</v>
       </c>
@@ -9655,7 +9131,7 @@
         <v>746</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="I185" s="1">
         <v>0</v>
@@ -9675,16 +9151,16 @@
         <v>747</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>986</v>
+        <v>919</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>987</v>
+        <v>981</v>
       </c>
       <c r="I186" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" ht="176" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>297</v>
       </c>
@@ -9698,10 +9174,10 @@
         <v>817</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>988</v>
+        <v>920</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>989</v>
+        <v>981</v>
       </c>
       <c r="I187" s="1">
         <v>0</v>
@@ -9741,7 +9217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="320" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>298</v>
       </c>
@@ -9755,13 +9231,13 @@
         <v>750</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>990</v>
+        <v>921</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>991</v>
+        <v>922</v>
       </c>
       <c r="G190" s="1" t="s">
-        <v>992</v>
+        <v>981</v>
       </c>
       <c r="I190" s="1">
         <v>0</v>
@@ -9798,7 +9274,7 @@
         <v>751</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>993</v>
+        <v>923</v>
       </c>
       <c r="I192" s="1">
         <v>0</v>
@@ -9818,13 +9294,13 @@
         <v>752</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>994</v>
+        <v>924</v>
       </c>
       <c r="I193" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>300</v>
       </c>
@@ -9838,7 +9314,7 @@
         <v>753</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>995</v>
+        <v>981</v>
       </c>
       <c r="I194" s="1">
         <v>0</v>
@@ -9858,7 +9334,7 @@
         <v>754</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>996</v>
+        <v>925</v>
       </c>
       <c r="I195" s="1">
         <v>0</v>
@@ -9895,7 +9371,7 @@
         <v>756</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>997</v>
+        <v>926</v>
       </c>
       <c r="I197" s="1">
         <v>0</v>
@@ -9966,7 +9442,7 @@
         <v>760</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>998</v>
+        <v>927</v>
       </c>
       <c r="I201" s="1">
         <v>0</v>
@@ -10023,7 +9499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="240" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:9" ht="208" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>307</v>
       </c>
@@ -10037,16 +9513,16 @@
         <v>763</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>999</v>
+        <v>928</v>
       </c>
       <c r="G205" s="1" t="s">
-        <v>1000</v>
+        <v>981</v>
       </c>
       <c r="I205" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="208" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:9" ht="240" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>308</v>
       </c>
@@ -10060,16 +9536,16 @@
         <v>764</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>1001</v>
+        <v>929</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>1002</v>
+        <v>981</v>
       </c>
       <c r="I206" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="350" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>309</v>
       </c>
@@ -10083,19 +9559,19 @@
         <v>765</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>1003</v>
+        <v>930</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>1004</v>
+        <v>931</v>
       </c>
       <c r="G207" s="1" t="s">
-        <v>1005</v>
+        <v>981</v>
       </c>
       <c r="I207" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="288" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>310</v>
       </c>
@@ -10109,13 +9585,13 @@
         <v>766</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>1006</v>
+        <v>932</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>1007</v>
+        <v>933</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>1008</v>
+        <v>981</v>
       </c>
       <c r="I208" s="1">
         <v>0</v>
@@ -10169,7 +9645,7 @@
         <v>769</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>1009</v>
+        <v>934</v>
       </c>
       <c r="I211" s="1">
         <v>0</v>
@@ -10189,7 +9665,7 @@
         <v>770</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>1009</v>
+        <v>934</v>
       </c>
       <c r="I212" s="1">
         <v>0</v>
@@ -10209,7 +9685,7 @@
         <v>771</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>1010</v>
+        <v>935</v>
       </c>
       <c r="I213" s="1">
         <v>0</v>
@@ -10229,10 +9705,10 @@
         <v>820</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>1011</v>
+        <v>936</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>1012</v>
+        <v>937</v>
       </c>
       <c r="I214" s="1">
         <v>0</v>
@@ -10252,7 +9728,7 @@
         <v>772</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>1013</v>
+        <v>938</v>
       </c>
       <c r="I215" s="1">
         <v>0</v>
@@ -10272,7 +9748,7 @@
         <v>821</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>1014</v>
+        <v>939</v>
       </c>
       <c r="I216" s="1">
         <v>0</v>
@@ -10326,7 +9802,7 @@
         <v>823</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>1014</v>
+        <v>939</v>
       </c>
       <c r="I219" s="1">
         <v>0</v>
@@ -10383,7 +9859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:9" ht="224" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>320</v>
       </c>
@@ -10397,13 +9873,13 @@
         <v>776</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>1015</v>
+        <v>940</v>
       </c>
       <c r="F223" s="1" t="s">
-        <v>1016</v>
+        <v>941</v>
       </c>
       <c r="G223" s="1" t="s">
-        <v>1017</v>
+        <v>981</v>
       </c>
       <c r="I223" s="1">
         <v>0</v>
@@ -10423,19 +9899,19 @@
         <v>824</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>1018</v>
+        <v>942</v>
       </c>
       <c r="F224" s="1" t="s">
-        <v>1019</v>
+        <v>943</v>
       </c>
       <c r="G224" s="1" t="s">
-        <v>1020</v>
+        <v>981</v>
       </c>
       <c r="I224" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:9" ht="256" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>322</v>
       </c>
@@ -10449,13 +9925,13 @@
         <v>777</v>
       </c>
       <c r="G225" s="1" t="s">
-        <v>1021</v>
+        <v>981</v>
       </c>
       <c r="I225" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:9" ht="224" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>323</v>
       </c>
@@ -10469,16 +9945,16 @@
         <v>842</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>1038</v>
+        <v>952</v>
       </c>
       <c r="G226" s="1" t="s">
-        <v>1022</v>
+        <v>981</v>
       </c>
       <c r="I226" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:9" ht="224" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>324</v>
       </c>
@@ -10492,16 +9968,16 @@
         <v>842</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>1023</v>
+        <v>944</v>
       </c>
       <c r="G227" s="1" t="s">
-        <v>1024</v>
+        <v>981</v>
       </c>
       <c r="I227" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>325</v>
       </c>
@@ -10515,16 +9991,16 @@
         <v>778</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>1038</v>
+        <v>952</v>
       </c>
       <c r="G228" s="1" t="s">
-        <v>1025</v>
+        <v>981</v>
       </c>
       <c r="I228" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" ht="256" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>326</v>
       </c>
@@ -10538,16 +10014,16 @@
         <v>779</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>1023</v>
+        <v>944</v>
       </c>
       <c r="G229" s="1" t="s">
-        <v>1026</v>
+        <v>981</v>
       </c>
       <c r="I229" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" ht="304" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>327</v>
       </c>
@@ -10561,16 +10037,16 @@
         <v>780</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>1038</v>
+        <v>952</v>
       </c>
       <c r="G230" s="1" t="s">
-        <v>1027</v>
+        <v>981</v>
       </c>
       <c r="I230" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="240" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>328</v>
       </c>
@@ -10584,10 +10060,10 @@
         <v>781</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>1023</v>
+        <v>944</v>
       </c>
       <c r="G231" s="1" t="s">
-        <v>1028</v>
+        <v>981</v>
       </c>
       <c r="I231" s="1">
         <v>0</v>
@@ -10627,7 +10103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9" ht="176" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>331</v>
       </c>
@@ -10641,16 +10117,16 @@
         <v>784</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>1039</v>
+        <v>953</v>
       </c>
       <c r="G234" s="1" t="s">
-        <v>1029</v>
+        <v>981</v>
       </c>
       <c r="I234" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9" ht="272" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>332</v>
       </c>
@@ -10667,7 +10143,7 @@
         <v>845</v>
       </c>
       <c r="G235" s="1" t="s">
-        <v>1030</v>
+        <v>981</v>
       </c>
       <c r="I235" s="1">
         <v>0</v>
@@ -10704,7 +10180,7 @@
         <v>787</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>1031</v>
+        <v>945</v>
       </c>
       <c r="I237" s="1">
         <v>0</v>
@@ -10724,7 +10200,7 @@
         <v>788</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>1032</v>
+        <v>946</v>
       </c>
       <c r="I238" s="1">
         <v>1</v>
@@ -10741,10 +10217,10 @@
         <v>175</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>1041</v>
+        <v>955</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>1058</v>
+        <v>972</v>
       </c>
       <c r="I239" s="1">
         <v>0</v>
@@ -10761,7 +10237,7 @@
         <v>501</v>
       </c>
       <c r="D240" s="5" t="s">
-        <v>1042</v>
+        <v>956</v>
       </c>
       <c r="I240" s="1">
         <v>0</v>
@@ -10778,7 +10254,7 @@
         <v>502</v>
       </c>
       <c r="D241" s="5" t="s">
-        <v>1043</v>
+        <v>957</v>
       </c>
       <c r="I241" s="1">
         <v>0</v>
@@ -10795,10 +10271,10 @@
         <v>503</v>
       </c>
       <c r="D242" s="4" t="s">
-        <v>1053</v>
+        <v>967</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>1059</v>
+        <v>973</v>
       </c>
       <c r="I242" s="1">
         <v>0</v>
@@ -10815,10 +10291,10 @@
         <v>504</v>
       </c>
       <c r="D243" s="4" t="s">
-        <v>1044</v>
+        <v>958</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>1064</v>
+        <v>978</v>
       </c>
       <c r="I243" s="1">
         <v>0</v>
@@ -10835,10 +10311,10 @@
         <v>505</v>
       </c>
       <c r="D244" s="4" t="s">
-        <v>1045</v>
+        <v>959</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>1064</v>
+        <v>978</v>
       </c>
       <c r="I244" s="1">
         <v>0</v>
@@ -10855,10 +10331,10 @@
         <v>506</v>
       </c>
       <c r="D245" s="4" t="s">
-        <v>1046</v>
+        <v>960</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>1060</v>
+        <v>974</v>
       </c>
       <c r="I245" s="1">
         <v>0</v>
@@ -10875,7 +10351,7 @@
         <v>507</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>1047</v>
+        <v>961</v>
       </c>
       <c r="I246" s="1">
         <v>0</v>
@@ -10892,7 +10368,7 @@
         <v>612</v>
       </c>
       <c r="D247" s="4" t="s">
-        <v>1054</v>
+        <v>968</v>
       </c>
       <c r="I247" s="1">
         <v>0</v>
@@ -10909,7 +10385,7 @@
         <v>508</v>
       </c>
       <c r="D248" s="4" t="s">
-        <v>1048</v>
+        <v>962</v>
       </c>
       <c r="I248" s="1">
         <v>0</v>
@@ -10926,7 +10402,7 @@
         <v>509</v>
       </c>
       <c r="D249" s="4" t="s">
-        <v>1049</v>
+        <v>963</v>
       </c>
       <c r="I249" s="1">
         <v>0</v>
@@ -10943,10 +10419,10 @@
         <v>510</v>
       </c>
       <c r="D250" s="4" t="s">
-        <v>1055</v>
+        <v>969</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>1061</v>
+        <v>975</v>
       </c>
       <c r="I250" s="1">
         <v>0</v>
@@ -10963,7 +10439,7 @@
         <v>511</v>
       </c>
       <c r="D251" s="6" t="s">
-        <v>1056</v>
+        <v>970</v>
       </c>
       <c r="I251" s="1">
         <v>0</v>
@@ -10980,7 +10456,7 @@
         <v>512</v>
       </c>
       <c r="D252" s="4" t="s">
-        <v>1057</v>
+        <v>971</v>
       </c>
       <c r="I252" s="1">
         <v>0</v>
@@ -10997,7 +10473,7 @@
         <v>513</v>
       </c>
       <c r="D253" s="4" t="s">
-        <v>1050</v>
+        <v>964</v>
       </c>
       <c r="I253" s="1">
         <v>0</v>
@@ -11014,10 +10490,10 @@
         <v>514</v>
       </c>
       <c r="D254" s="6" t="s">
-        <v>1051</v>
+        <v>965</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>1062</v>
+        <v>976</v>
       </c>
       <c r="I254" s="1">
         <v>0</v>
@@ -11034,10 +10510,10 @@
         <v>515</v>
       </c>
       <c r="D255" s="6" t="s">
-        <v>1052</v>
+        <v>966</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>1063</v>
+        <v>977</v>
       </c>
       <c r="I255" s="1">
         <v>0</v>

</xml_diff>